<commit_message>
update quick start generator to show composites
</commit_message>
<xml_diff>
--- a/SP/uscore-client.xlsx
+++ b/SP/uscore-client.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric\Documents\Python\MyNotebooks\SP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/Python/MyNotebooks/SP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6271381-46EA-4B5A-AF5D-E1B928EB5302}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41F34314-A189-AD4B-BF93-9895015E571E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-68805" yWindow="-10800" windowWidth="68805" windowHeight="28800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="1" r:id="rId1"/>
@@ -32,6 +32,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -52,7 +53,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>User:</t>
         </r>
@@ -61,7 +62,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 not used -for algorithmic generation of combos</t>
@@ -86,7 +87,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>User:</t>
         </r>
@@ -95,7 +96,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 not being used since enumerating for US Core</t>
@@ -107,7 +108,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1912" uniqueCount="496">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1913" uniqueCount="497">
   <si>
     <t>Element</t>
   </si>
@@ -1603,13 +1604,16 @@
   </si>
   <si>
     <t>us-core-client</t>
+  </si>
+  <si>
+    <t>The DocumentReference.type binding SHALL support at a minimum the [5 Common Clinical Notes](ValueSet-us-core-clinical-note-type.html) and may extend to the full US Core DocumentReference Type Value Set</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1659,14 +1663,14 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
@@ -2071,17 +2075,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="95.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="95.5" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2089,7 +2093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2097,7 +2101,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="105" customHeight="1">
+    <row r="3" spans="1:2" ht="105" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -2105,13 +2109,13 @@
         <v>487</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="11"/>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -2119,7 +2123,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="141" customHeight="1">
+    <row r="6" spans="1:2" ht="141" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -2127,7 +2131,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="103.5" customHeight="1">
+    <row r="7" spans="1:2" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -2148,9 +2152,9 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -2167,19 +2171,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="B28" sqref="B28:B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="94" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="60.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="60.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -2193,7 +2197,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>400</v>
       </c>
@@ -2208,7 +2212,7 @@
       </c>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>402</v>
       </c>
@@ -2223,7 +2227,7 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>404</v>
       </c>
@@ -2238,7 +2242,7 @@
       </c>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>405</v>
       </c>
@@ -2253,7 +2257,7 @@
       </c>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>86</v>
       </c>
@@ -2268,7 +2272,7 @@
       </c>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>407</v>
       </c>
@@ -2283,7 +2287,7 @@
       </c>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>319</v>
       </c>
@@ -2298,7 +2302,7 @@
       </c>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>410</v>
       </c>
@@ -2313,7 +2317,7 @@
       </c>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>412</v>
       </c>
@@ -2328,7 +2332,7 @@
       </c>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>414</v>
       </c>
@@ -2343,7 +2347,7 @@
       </c>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>416</v>
       </c>
@@ -2358,7 +2362,7 @@
       </c>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>417</v>
       </c>
@@ -2373,7 +2377,7 @@
       </c>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>419</v>
       </c>
@@ -2388,7 +2392,7 @@
       </c>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>420</v>
       </c>
@@ -2403,7 +2407,7 @@
       </c>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>422</v>
       </c>
@@ -2418,7 +2422,7 @@
       </c>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>208</v>
       </c>
@@ -2433,7 +2437,7 @@
       </c>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>209</v>
       </c>
@@ -2448,7 +2452,7 @@
       </c>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>427</v>
       </c>
@@ -2463,7 +2467,7 @@
       </c>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>270</v>
       </c>
@@ -2478,7 +2482,7 @@
       </c>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>430</v>
       </c>
@@ -2493,7 +2497,7 @@
       </c>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>432</v>
       </c>
@@ -2508,7 +2512,7 @@
       </c>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>434</v>
       </c>
@@ -2523,7 +2527,7 @@
       </c>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>207</v>
       </c>
@@ -2538,7 +2542,7 @@
       </c>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>84</v>
       </c>
@@ -2567,15 +2571,15 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="89" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" customWidth="1"/>
-    <col min="3" max="3" width="59.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="3" max="3" width="59.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -2589,7 +2593,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -2603,7 +2607,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -2617,7 +2621,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -2631,7 +2635,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -2645,7 +2649,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -2659,7 +2663,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -2673,7 +2677,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -2687,7 +2691,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -2701,7 +2705,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>13</v>
       </c>
@@ -2712,7 +2716,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>13</v>
       </c>
@@ -2723,7 +2727,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
@@ -2734,7 +2738,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
         <v>13</v>
       </c>
@@ -2745,7 +2749,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
         <v>13</v>
       </c>
@@ -2756,7 +2760,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
         <v>13</v>
       </c>
@@ -2767,7 +2771,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
         <v>13</v>
       </c>
@@ -2778,7 +2782,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="17" spans="2:4">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
         <v>13</v>
       </c>
@@ -2789,7 +2793,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="18" spans="2:4">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
         <v>13</v>
       </c>
@@ -2800,7 +2804,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="19" spans="2:4">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
         <v>13</v>
       </c>
@@ -2811,7 +2815,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="20" spans="2:4">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
         <v>13</v>
       </c>
@@ -2822,7 +2826,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="21" spans="2:4">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
         <v>13</v>
       </c>
@@ -2833,7 +2837,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="22" spans="2:4">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
         <v>13</v>
       </c>
@@ -2844,7 +2848,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="23" spans="2:4">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
         <v>13</v>
       </c>
@@ -2855,7 +2859,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="24" spans="2:4">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
         <v>13</v>
       </c>
@@ -2866,7 +2870,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="25" spans="2:4">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
         <v>13</v>
       </c>
@@ -2887,28 +2891,28 @@
   <dimension ref="A1:X59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="V2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="X1" sqref="X1"/>
+      <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="17.25" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="36.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="49.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="36.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="49.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="1" customWidth="1"/>
-    <col min="6" max="12" width="17.42578125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="20.5703125" style="1" customWidth="1"/>
-    <col min="14" max="17" width="17.42578125" style="1" customWidth="1"/>
-    <col min="18" max="19" width="20.42578125" style="1" customWidth="1"/>
-    <col min="20" max="23" width="38.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="27.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="12" width="17.5" style="1" customWidth="1"/>
+    <col min="13" max="13" width="20.5" style="1" customWidth="1"/>
+    <col min="14" max="17" width="17.5" style="1" customWidth="1"/>
+    <col min="18" max="19" width="20.5" style="1" customWidth="1"/>
+    <col min="20" max="23" width="38.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="27.1640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="17.25" customHeight="1" thickBot="1">
+    <row r="1" spans="1:24" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -2982,7 +2986,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="17.25" customHeight="1" thickTop="1">
+    <row r="2" spans="1:24" ht="17.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>29</v>
       </c>
@@ -2997,7 +3001,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="17.25" customHeight="1">
+    <row r="3" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>268</v>
       </c>
@@ -3005,7 +3009,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:24" ht="17.25" customHeight="1">
+    <row r="4" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>284</v>
       </c>
@@ -3013,7 +3017,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:24" ht="17.25" customHeight="1">
+    <row r="5" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>151</v>
       </c>
@@ -3024,7 +3028,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:24" ht="17.25" customHeight="1">
+    <row r="6" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>288</v>
       </c>
@@ -3032,7 +3036,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:24" ht="17.25" customHeight="1">
+    <row r="7" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>195</v>
       </c>
@@ -3040,15 +3044,18 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:24" ht="17.25" customHeight="1">
+    <row r="8" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>194</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="9" spans="1:24" ht="17.25" customHeight="1">
+      <c r="C8" s="2" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>31</v>
       </c>
@@ -3056,7 +3063,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="10" spans="1:24" ht="17.25" customHeight="1">
+    <row r="10" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>196</v>
       </c>
@@ -3064,7 +3071,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:24" ht="17.25" customHeight="1">
+    <row r="11" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>175</v>
       </c>
@@ -3072,7 +3079,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:24" ht="17.25" customHeight="1">
+    <row r="12" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>289</v>
       </c>
@@ -3080,7 +3087,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:24" ht="17.25" customHeight="1">
+    <row r="13" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>424</v>
       </c>
@@ -3091,7 +3098,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="14" spans="1:24" ht="17.25" customHeight="1">
+    <row r="14" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>197</v>
       </c>
@@ -3105,7 +3112,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="15" spans="1:24" ht="17.25" customHeight="1">
+    <row r="15" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>200</v>
       </c>
@@ -3119,7 +3126,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="16" spans="1:24" ht="17.25" customHeight="1">
+    <row r="16" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>199</v>
       </c>
@@ -3127,7 +3134,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="17" spans="1:21" ht="17.25" customHeight="1">
+    <row r="17" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>303</v>
       </c>
@@ -3135,7 +3142,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="1:21" ht="17.25" customHeight="1">
+    <row r="18" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>30</v>
       </c>
@@ -3143,7 +3150,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="19" spans="1:21" ht="17.25" customHeight="1">
+    <row r="19" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>310</v>
       </c>
@@ -3151,7 +3158,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:21" ht="17.25" customHeight="1">
+    <row r="20" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>313</v>
       </c>
@@ -3162,7 +3169,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="21" spans="1:21" ht="17.25" customHeight="1">
+    <row r="21" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>198</v>
       </c>
@@ -3170,28 +3177,28 @@
         <v>81</v>
       </c>
     </row>
-    <row r="22" spans="1:21" ht="17.25" customHeight="1">
+    <row r="22" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22"/>
     </row>
-    <row r="23" spans="1:21" ht="17.25" customHeight="1">
+    <row r="23" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23"/>
     </row>
-    <row r="24" spans="1:21" ht="17.25" customHeight="1">
+    <row r="24" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24"/>
     </row>
-    <row r="25" spans="1:21" ht="17.25" customHeight="1">
+    <row r="25" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25"/>
     </row>
-    <row r="56" spans="20:23" ht="17.25" customHeight="1">
+    <row r="56" spans="20:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="T56" s="7"/>
       <c r="V56" s="7"/>
       <c r="W56" s="7"/>
     </row>
-    <row r="59" spans="20:23" ht="17.25" customHeight="1">
+    <row r="59" spans="20:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="W59" s="7"/>
     </row>
   </sheetData>
-  <sortState ref="A2:A21">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A21">
     <sortCondition ref="A2:A21"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3208,15 +3215,15 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" customWidth="1"/>
     <col min="5" max="5" width="89" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1">
+    <row r="1" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -3233,7 +3240,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="120.75" thickBot="1">
+    <row r="2" spans="1:5" ht="113" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>442</v>
       </c>
@@ -3250,7 +3257,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E4" s="2"/>
     </row>
   </sheetData>
@@ -3266,15 +3273,15 @@
       <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.83203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="15" style="1" customWidth="1"/>
-    <col min="8" max="8" width="28.140625" customWidth="1"/>
+    <col min="8" max="8" width="28.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -3339,7 +3346,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -3404,7 +3411,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -3469,7 +3476,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -3534,7 +3541,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>41</v>
       </c>
@@ -3599,7 +3606,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -3664,7 +3671,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -3729,7 +3736,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>44</v>
       </c>
@@ -3794,7 +3801,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -3859,7 +3866,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -3940,34 +3947,34 @@
       <selection pane="bottomRight" activeCell="U60" sqref="U60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="1"/>
-    <col min="2" max="2" width="21.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="1"/>
+    <col min="2" max="2" width="21.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="36.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="36.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.1640625" style="1" customWidth="1"/>
     <col min="12" max="12" width="11" style="1" customWidth="1"/>
-    <col min="13" max="13" width="12.7109375" style="1" customWidth="1"/>
-    <col min="14" max="14" width="10.28515625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="16.28515625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="12.6640625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="10.33203125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="16.33203125" style="1" customWidth="1"/>
     <col min="16" max="16" width="18" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="21.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="49.7109375" style="1" customWidth="1"/>
-    <col min="21" max="22" width="38.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="49.6640625" style="1" customWidth="1"/>
+    <col min="21" max="22" width="38.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="16" style="1" customWidth="1"/>
-    <col min="24" max="24" width="50.85546875" style="1" customWidth="1"/>
-    <col min="25" max="25" width="68.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="90.7109375" style="1" customWidth="1"/>
-    <col min="27" max="27" width="83.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="38.140625" customWidth="1"/>
+    <col min="24" max="24" width="50.83203125" style="1" customWidth="1"/>
+    <col min="25" max="25" width="68.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="90.6640625" style="1" customWidth="1"/>
+    <col min="27" max="27" width="83.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="38.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="18" customHeight="1" thickBot="1">
+    <row r="1" spans="1:28" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>154</v>
       </c>
@@ -4053,7 +4060,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="2" spans="1:28" s="1" customFormat="1" ht="15.75" thickTop="1">
+    <row r="2" spans="1:28" s="1" customFormat="1" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -4103,7 +4110,7 @@
         <v>SearchParameter-us-core-!example category search-category.html</v>
       </c>
     </row>
-    <row r="3" spans="1:28" s="1" customFormat="1">
+    <row r="3" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -4150,7 +4157,7 @@
         <v>SearchParameter-us-core-!example code search-code.html</v>
       </c>
     </row>
-    <row r="4" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="4" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -4204,7 +4211,7 @@
         <v>SearchParameter-us-core-!example date search-date.html</v>
       </c>
     </row>
-    <row r="5" spans="1:28" s="1" customFormat="1" ht="29.25">
+    <row r="5" spans="1:28" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -4263,7 +4270,7 @@
         <v>SearchParameter-us-core-!example patient search-patient.html</v>
       </c>
     </row>
-    <row r="6" spans="1:28" s="1" customFormat="1">
+    <row r="6" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -4313,7 +4320,7 @@
         <v>SearchParameter-us-core-!example status search-status.html</v>
       </c>
     </row>
-    <row r="7" spans="1:28" ht="15.75" customHeight="1">
+    <row r="7" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -4363,7 +4370,7 @@
         <v>SearchParameter-us-core-!patient-address.html</v>
       </c>
     </row>
-    <row r="8" spans="1:28">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -4413,7 +4420,7 @@
         <v>SearchParameter-us-core-!patient-telecom.html</v>
       </c>
     </row>
-    <row r="9" spans="1:28">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -4459,7 +4466,7 @@
         <v>SearchParameter-us-core-allergyintolerance-clinical-status.html</v>
       </c>
     </row>
-    <row r="10" spans="1:28" ht="29.25">
+    <row r="10" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -4518,7 +4525,7 @@
         <v>SearchParameter-us-core-allergyintolerance-patient.html</v>
       </c>
     </row>
-    <row r="11" spans="1:28">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -4569,7 +4576,7 @@
         <v>SearchParameter-us-core-condition-category.html</v>
       </c>
     </row>
-    <row r="12" spans="1:28">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -4617,7 +4624,7 @@
         <v>SearchParameter-us-core-condition-clinical-status.html</v>
       </c>
     </row>
-    <row r="13" spans="1:28">
+    <row r="13" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -4675,7 +4682,7 @@
         <v>SearchParameter-us-core-condition-patient.html</v>
       </c>
     </row>
-    <row r="14" spans="1:28" ht="15.75" customHeight="1">
+    <row r="14" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -4728,7 +4735,7 @@
         <v>SearchParameter-us-core-encounter-id.html</v>
       </c>
     </row>
-    <row r="15" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="15" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -4778,7 +4785,7 @@
         <v>SearchParameter-us-core-encounter-class.html</v>
       </c>
     </row>
-    <row r="16" spans="1:28" ht="15.75" customHeight="1">
+    <row r="16" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -4832,7 +4839,7 @@
         <v>SearchParameter-us-core-encounter-date.html</v>
       </c>
     </row>
-    <row r="17" spans="1:28" ht="29.25">
+    <row r="17" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -4886,7 +4893,7 @@
         <v>SearchParameter-us-core-encounter-identifier.html</v>
       </c>
     </row>
-    <row r="18" spans="1:28">
+    <row r="18" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -4944,7 +4951,7 @@
         <v>SearchParameter-us-core-encounter-patient.html</v>
       </c>
     </row>
-    <row r="19" spans="1:28">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -4994,7 +5001,7 @@
         <v>SearchParameter-us-core-encounter-status.html</v>
       </c>
     </row>
-    <row r="20" spans="1:28">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -5042,7 +5049,7 @@
         <v>SearchParameter-us-core-encounter-type.html</v>
       </c>
     </row>
-    <row r="21" spans="1:28">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -5092,7 +5099,7 @@
         <v>SearchParameter-us-core-patient-id.html</v>
       </c>
     </row>
-    <row r="22" spans="1:28">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -5143,7 +5150,7 @@
         <v>SearchParameter-us-core-patient-birthdate.html</v>
       </c>
     </row>
-    <row r="23" spans="1:28">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -5187,7 +5194,7 @@
         <v>SearchParameter-us-core-patient-family.html</v>
       </c>
     </row>
-    <row r="24" spans="1:28">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -5236,7 +5243,7 @@
         <v>SearchParameter-us-core-patient-gender.html</v>
       </c>
     </row>
-    <row r="25" spans="1:28" ht="15.75" customHeight="1">
+    <row r="25" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -5280,7 +5287,7 @@
         <v>SearchParameter-us-core-patient-given.html</v>
       </c>
     </row>
-    <row r="26" spans="1:28" ht="15.75" customHeight="1">
+    <row r="26" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -5335,7 +5342,7 @@
         <v>SearchParameter-us-core-patient-identifier.html</v>
       </c>
     </row>
-    <row r="27" spans="1:28" ht="15.75" customHeight="1">
+    <row r="27" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -5393,7 +5400,7 @@
         <v>SearchParameter-us-core-patient-name.html</v>
       </c>
     </row>
-    <row r="28" spans="1:28">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -5436,7 +5443,7 @@
         <v>SearchParameter-us-core-!questionnaire-_id.html</v>
       </c>
     </row>
-    <row r="29" spans="1:28" ht="15.75" customHeight="1">
+    <row r="29" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -5481,7 +5488,7 @@
         <v>SearchParameter-us-core-!questionnaire-context-type-value.html</v>
       </c>
     </row>
-    <row r="30" spans="1:28" ht="15.75" customHeight="1">
+    <row r="30" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -5531,7 +5538,7 @@
         <v>SearchParameter-us-core-!questionnaire-publisher.html</v>
       </c>
     </row>
-    <row r="31" spans="1:28" ht="15.75" customHeight="1">
+    <row r="31" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -5578,7 +5585,7 @@
         <v>SearchParameter-us-core-!questionnaire-status.html</v>
       </c>
     </row>
-    <row r="32" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="32" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -5638,7 +5645,7 @@
         <v>SearchParameter-us-core-!questionnaire-title.html</v>
       </c>
     </row>
-    <row r="33" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="33" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -5683,7 +5690,7 @@
         <v>SearchParameter-us-core-!questionnaire-url.html</v>
       </c>
     </row>
-    <row r="34" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="34" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -5728,7 +5735,7 @@
         <v>SearchParameter-us-core-!questionnaire-version.html</v>
       </c>
     </row>
-    <row r="35" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="35" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -5779,7 +5786,7 @@
         <v>SearchParameter-us-core-condition-onset-date.html</v>
       </c>
     </row>
-    <row r="36" spans="1:28" s="1" customFormat="1">
+    <row r="36" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -5826,7 +5833,7 @@
         <v>SearchParameter-us-core-condition-code.html</v>
       </c>
     </row>
-    <row r="37" spans="1:28" s="1" customFormat="1">
+    <row r="37" spans="1:28" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -5885,7 +5892,7 @@
         <v>SearchParameter-us-core-immunization-patient.html</v>
       </c>
     </row>
-    <row r="38" spans="1:28" s="1" customFormat="1">
+    <row r="38" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -5935,7 +5942,7 @@
         <v>SearchParameter-us-core-immunization-status.html</v>
       </c>
     </row>
-    <row r="39" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="39" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -5989,7 +5996,7 @@
         <v>SearchParameter-us-core-immunization-date.html</v>
       </c>
     </row>
-    <row r="40" spans="1:28" s="1" customFormat="1" ht="60">
+    <row r="40" spans="1:28" s="1" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -6042,7 +6049,7 @@
         <v>SearchParameter-us-core-documentreference-_id.html</v>
       </c>
     </row>
-    <row r="41" spans="1:28" s="1" customFormat="1">
+    <row r="41" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -6092,7 +6099,7 @@
         <v>SearchParameter-us-core-documentreference-status.html</v>
       </c>
     </row>
-    <row r="42" spans="1:28" s="1" customFormat="1" ht="43.5">
+    <row r="42" spans="1:28" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -6151,7 +6158,7 @@
         <v>SearchParameter-us-core-documentreference-patient.html</v>
       </c>
     </row>
-    <row r="43" spans="1:28" s="1" customFormat="1">
+    <row r="43" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -6201,7 +6208,7 @@
         <v>SearchParameter-us-core-documentreference-category.html</v>
       </c>
     </row>
-    <row r="44" spans="1:28" s="1" customFormat="1">
+    <row r="44" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -6248,7 +6255,7 @@
         <v>SearchParameter-us-core-documentreference-type.html</v>
       </c>
     </row>
-    <row r="45" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="45" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -6302,7 +6309,7 @@
         <v>SearchParameter-us-core-documentreference-date.html</v>
       </c>
     </row>
-    <row r="46" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="46" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -6355,7 +6362,7 @@
         <v>SearchParameter-us-core-documentreference-period.html</v>
       </c>
     </row>
-    <row r="47" spans="1:28" s="1" customFormat="1">
+    <row r="47" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -6405,7 +6412,7 @@
         <v>SearchParameter-us-core-diagnosticreport-status.html</v>
       </c>
     </row>
-    <row r="48" spans="1:28" s="1" customFormat="1">
+    <row r="48" spans="1:28" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -6464,7 +6471,7 @@
         <v>SearchParameter-us-core-diagnosticreport-patient.html</v>
       </c>
     </row>
-    <row r="49" spans="1:28" s="1" customFormat="1">
+    <row r="49" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -6514,7 +6521,7 @@
         <v>SearchParameter-us-core-diagnosticreport-category.html</v>
       </c>
     </row>
-    <row r="50" spans="1:28" s="1" customFormat="1">
+    <row r="50" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -6564,7 +6571,7 @@
         <v>SearchParameter-us-core-diagnosticreport-code.html</v>
       </c>
     </row>
-    <row r="51" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="51" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -6618,7 +6625,7 @@
         <v>SearchParameter-us-core-diagnosticreport-date.html</v>
       </c>
     </row>
-    <row r="52" spans="1:28" s="1" customFormat="1">
+    <row r="52" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -6668,7 +6675,7 @@
         <v>SearchParameter-us-core-goal-lifecycle-status.html</v>
       </c>
     </row>
-    <row r="53" spans="1:28" s="1" customFormat="1">
+    <row r="53" spans="1:28" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -6727,7 +6734,7 @@
         <v>SearchParameter-us-core-goal-patient.html</v>
       </c>
     </row>
-    <row r="54" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="54" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -6781,7 +6788,7 @@
         <v>SearchParameter-us-core-goal-start-date.html</v>
       </c>
     </row>
-    <row r="55" spans="1:28" s="1" customFormat="1">
+    <row r="55" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -6831,7 +6838,7 @@
         <v>SearchParameter-us-core-medicationrequest-status.html</v>
       </c>
     </row>
-    <row r="56" spans="1:28" s="1" customFormat="1" ht="43.5">
+    <row r="56" spans="1:28" s="1" customFormat="1" ht="46" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -6892,7 +6899,7 @@
         <v>SearchParameter-us-core-medicationrequest-patient.html</v>
       </c>
     </row>
-    <row r="57" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="57" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -6946,7 +6953,7 @@
         <v>SearchParameter-us-core-medicationrequest-authoredon.html</v>
       </c>
     </row>
-    <row r="58" spans="1:28" s="1" customFormat="1">
+    <row r="58" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -6996,7 +7003,7 @@
         <v>SearchParameter-us-core-medicationstatement-status.html</v>
       </c>
     </row>
-    <row r="59" spans="1:28" s="1" customFormat="1" ht="43.5">
+    <row r="59" spans="1:28" s="1" customFormat="1" ht="46" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -7056,7 +7063,7 @@
         <v>SearchParameter-us-core-medicationstatement-patient.html</v>
       </c>
     </row>
-    <row r="60" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="60" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -7110,7 +7117,7 @@
         <v>SearchParameter-us-core-medicationstatement-effective.html</v>
       </c>
     </row>
-    <row r="61" spans="1:28" s="1" customFormat="1">
+    <row r="61" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -7160,7 +7167,7 @@
         <v>SearchParameter-us-core-procedure-status.html</v>
       </c>
     </row>
-    <row r="62" spans="1:28" s="1" customFormat="1">
+    <row r="62" spans="1:28" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -7218,7 +7225,7 @@
         <v>SearchParameter-us-core-procedure-patient.html</v>
       </c>
     </row>
-    <row r="63" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="63" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -7272,7 +7279,7 @@
         <v>SearchParameter-us-core-procedure-date.html</v>
       </c>
     </row>
-    <row r="64" spans="1:28" s="1" customFormat="1">
+    <row r="64" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -7322,7 +7329,7 @@
         <v>SearchParameter-us-core-procedure-code.html</v>
       </c>
     </row>
-    <row r="65" spans="1:28" s="1" customFormat="1">
+    <row r="65" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -7372,7 +7379,7 @@
         <v>SearchParameter-us-core-observation-status.html</v>
       </c>
     </row>
-    <row r="66" spans="1:28" s="1" customFormat="1">
+    <row r="66" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -7422,7 +7429,7 @@
         <v>SearchParameter-us-core-observation-category.html</v>
       </c>
     </row>
-    <row r="67" spans="1:28" s="1" customFormat="1">
+    <row r="67" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -7472,7 +7479,7 @@
         <v>SearchParameter-us-core-observation-code.html</v>
       </c>
     </row>
-    <row r="68" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="68" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -7526,7 +7533,7 @@
         <v>SearchParameter-us-core-observation-date.html</v>
       </c>
     </row>
-    <row r="69" spans="1:28" s="1" customFormat="1">
+    <row r="69" spans="1:28" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -7585,7 +7592,7 @@
         <v>SearchParameter-us-core-observation-patient.html</v>
       </c>
     </row>
-    <row r="70" spans="1:28" s="1" customFormat="1">
+    <row r="70" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -7635,7 +7642,7 @@
         <v>SearchParameter-us-core-careplan-category.html</v>
       </c>
     </row>
-    <row r="71" spans="1:28" s="1" customFormat="1">
+    <row r="71" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -7682,7 +7689,7 @@
         <v>SearchParameter-us-core-!careplan-code.html</v>
       </c>
     </row>
-    <row r="72" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="72" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -7736,7 +7743,7 @@
         <v>SearchParameter-us-core-careplan-date.html</v>
       </c>
     </row>
-    <row r="73" spans="1:28" s="1" customFormat="1">
+    <row r="73" spans="1:28" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -7795,7 +7802,7 @@
         <v>SearchParameter-us-core-careplan-patient.html</v>
       </c>
     </row>
-    <row r="74" spans="1:28" s="1" customFormat="1">
+    <row r="74" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -7845,7 +7852,7 @@
         <v>SearchParameter-us-core-careplan-status.html</v>
       </c>
     </row>
-    <row r="75" spans="1:28" s="1" customFormat="1">
+    <row r="75" spans="1:28" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -7904,7 +7911,7 @@
         <v>SearchParameter-us-core-careteam-patient.html</v>
       </c>
     </row>
-    <row r="76" spans="1:28" s="1" customFormat="1">
+    <row r="76" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -7954,7 +7961,7 @@
         <v>SearchParameter-us-core-careteam-status.html</v>
       </c>
     </row>
-    <row r="77" spans="1:28" s="1" customFormat="1">
+    <row r="77" spans="1:28" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -8013,7 +8020,7 @@
         <v>SearchParameter-us-core-device-patient.html</v>
       </c>
     </row>
-    <row r="78" spans="1:28" s="1" customFormat="1">
+    <row r="78" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -8055,7 +8062,7 @@
       <c r="Z78" s="5"/>
       <c r="AA78" s="12"/>
     </row>
-    <row r="79" spans="1:28" ht="18">
+    <row r="79" spans="1:28" ht="18" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -8109,7 +8116,7 @@
         <v>SearchParameter-us-core-location-name.html</v>
       </c>
     </row>
-    <row r="80" spans="1:28" ht="18">
+    <row r="80" spans="1:28" ht="18" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -8163,7 +8170,7 @@
         <v>SearchParameter-us-core-location-address.html</v>
       </c>
     </row>
-    <row r="81" spans="1:28" ht="18">
+    <row r="81" spans="1:28" ht="18" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -8217,7 +8224,7 @@
         <v>SearchParameter-us-core-location-address-city.html</v>
       </c>
     </row>
-    <row r="82" spans="1:28" ht="18">
+    <row r="82" spans="1:28" ht="18" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -8271,7 +8278,7 @@
         <v>SearchParameter-us-core-location-address-state.html</v>
       </c>
     </row>
-    <row r="83" spans="1:28" ht="18">
+    <row r="83" spans="1:28" ht="18" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -8325,7 +8332,7 @@
         <v>SearchParameter-us-core-location-address-postalcode.html</v>
       </c>
     </row>
-    <row r="84" spans="1:28" s="1" customFormat="1" ht="18">
+    <row r="84" spans="1:28" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -8379,7 +8386,7 @@
         <v>SearchParameter-us-core-organization-name.html</v>
       </c>
     </row>
-    <row r="85" spans="1:28" s="1" customFormat="1" ht="29.25">
+    <row r="85" spans="1:28" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -8433,7 +8440,7 @@
         <v>SearchParameter-us-core-organization-address.html</v>
       </c>
     </row>
-    <row r="86" spans="1:28" s="1" customFormat="1" ht="18">
+    <row r="86" spans="1:28" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -8487,7 +8494,7 @@
         <v>SearchParameter-us-core-!organization-address-city.html</v>
       </c>
     </row>
-    <row r="87" spans="1:28" s="1" customFormat="1" ht="18">
+    <row r="87" spans="1:28" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -8541,7 +8548,7 @@
         <v>SearchParameter-us-core-!organization-adress-state.html</v>
       </c>
     </row>
-    <row r="88" spans="1:28" s="1" customFormat="1" ht="18">
+    <row r="88" spans="1:28" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -8595,7 +8602,7 @@
         <v>SearchParameter-us-core-!organization-address-postalcode.html</v>
       </c>
     </row>
-    <row r="89" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="89" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -8652,7 +8659,7 @@
         <v>SearchParameter-us-core-practitioner-name.html</v>
       </c>
     </row>
-    <row r="90" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="90" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -8706,7 +8713,7 @@
         <v>SearchParameter-us-core-practitioner-identifier.html</v>
       </c>
     </row>
-    <row r="91" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="91" spans="1:28" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -8763,7 +8770,7 @@
         <v>SearchParameter-us-core-practitionerrole-specialty.html</v>
       </c>
     </row>
-    <row r="92" spans="1:28" ht="38.1" customHeight="1">
+    <row r="92" spans="1:28" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -8823,12 +8830,12 @@
         <v>SearchParameter-us-core-practitionerrole-practitioner.html</v>
       </c>
     </row>
-    <row r="93" spans="1:28">
+    <row r="93" spans="1:28" x14ac:dyDescent="0.2">
       <c r="Y93" s="5"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:AB92" xr:uid="{1CF5B17E-E72E-48B2-A597-9C21C12723F0}"/>
-  <sortState ref="A7:AA34">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:AA34">
     <sortCondition ref="B1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8841,28 +8848,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:P82"/>
   <sheetViews>
-    <sheetView zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="I71" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <pane xSplit="6" ySplit="1" topLeftCell="I42" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D87" sqref="D87"/>
+      <selection pane="bottomRight" activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="1"/>
-    <col min="2" max="2" width="21.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="1"/>
+    <col min="2" max="2" width="21.1640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="66" style="1" customWidth="1"/>
-    <col min="4" max="4" width="38.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27" style="1" customWidth="1"/>
-    <col min="8" max="8" width="84.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="68.28515625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="83.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="84.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="68.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="83.5" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" customHeight="1" thickBot="1">
+    <row r="1" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>156</v>
       </c>
@@ -8894,7 +8901,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1" thickTop="1">
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -8919,7 +8926,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and date</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -8944,7 +8951,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and date and patient</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -8969,7 +8976,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and date and patient and type</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -8994,7 +9001,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and date and type</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -9025,7 +9032,7 @@
         <v>Fetches a bundle of all Encounter resources matching the specified class and patient</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -9050,7 +9057,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and patient and status</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -9075,7 +9082,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and patient and status and type</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -9101,7 +9108,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and patient and type</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -9128,7 +9135,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and status</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -9154,7 +9161,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and status and type</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -9179,7 +9186,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and type</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -9210,7 +9217,7 @@
         <v>Fetches a bundle of all Encounter resources matching the specified date and patient</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -9235,7 +9242,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified date and patient and type</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -9260,7 +9267,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified date and type</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -9291,7 +9298,7 @@
         <v>Fetches a bundle of all Encounter resources matching the specified patient and type</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -9317,7 +9324,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified patient and status and type</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -9348,7 +9355,7 @@
         <v>Fetches a bundle of all Encounter resources matching the specified patient and status</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -9375,7 +9382,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified status and type</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -9401,7 +9408,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified context-type-value and publisher</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -9426,7 +9433,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified context-type-value and publisher and status</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -9452,7 +9459,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified context-type-value and status</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -9479,7 +9486,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified publisher and status</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -9506,7 +9513,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified publisher and status and version</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -9533,7 +9540,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified publisher and version</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -9558,7 +9565,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified status and title and version</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -9583,7 +9590,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified status and version</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -9608,7 +9615,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified title and version</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -9639,7 +9646,7 @@
         <v>Fetches a bundle of all Patient resources matching the specified birthdate and family</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -9670,7 +9677,7 @@
         <v>Fetches a bundle of all Patient resources matching the specified birthdate and name</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -9701,7 +9708,7 @@
         <v>Fetches a bundle of all Patient resources matching the specified family and gender</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -9732,7 +9739,7 @@
         <v>Fetches a bundle of all Patient resources matching the specified gender and name</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -9765,7 +9772,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -9795,7 +9802,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -9825,7 +9832,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="36" spans="1:10" s="1" customFormat="1">
+    <row r="36" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -9855,7 +9862,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -9885,7 +9892,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="38" spans="1:10" s="1" customFormat="1">
+    <row r="38" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -9916,7 +9923,7 @@
         <v>Fetches a bundle of all Immunization resources for the specified patient and date</v>
       </c>
     </row>
-    <row r="39" spans="1:10" s="1" customFormat="1">
+    <row r="39" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -9947,7 +9954,7 @@
         <v>Fetches a bundle of all Immunization resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="40" spans="1:10" s="1" customFormat="1">
+    <row r="40" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -9977,7 +9984,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="41" spans="1:10" s="1" customFormat="1" ht="15.75">
+    <row r="41" spans="1:10" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -10010,7 +10017,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and  a category code = `LAB`</v>
       </c>
     </row>
-    <row r="42" spans="1:10" s="1" customFormat="1" ht="15.75">
+    <row r="42" spans="1:10" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -10040,7 +10047,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="43" spans="1:10" s="1" customFormat="1" ht="15.75">
+    <row r="43" spans="1:10" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -10073,7 +10080,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and date and a category code = `LAB`</v>
       </c>
     </row>
-    <row r="44" spans="1:10" s="1" customFormat="1">
+    <row r="44" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -10103,7 +10110,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="45" spans="1:10" s="1" customFormat="1">
+    <row r="45" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -10133,7 +10140,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="46" spans="1:10" s="1" customFormat="1">
+    <row r="46" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -10163,7 +10170,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and  a category code specified in US Core DiagnosticReport Category Codes</v>
       </c>
     </row>
-    <row r="47" spans="1:10" s="1" customFormat="1">
+    <row r="47" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -10193,7 +10200,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="48" spans="1:10" s="1" customFormat="1">
+    <row r="48" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -10223,7 +10230,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and date and a category code specified in US Core DiagnosticReport Category Codes</v>
       </c>
     </row>
-    <row r="49" spans="1:10" s="1" customFormat="1">
+    <row r="49" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -10253,7 +10260,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="50" spans="1:10" s="1" customFormat="1">
+    <row r="50" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -10284,7 +10291,7 @@
         <v>Fetches a bundle of all Goal resources for the specified patient and lifecycle-status</v>
       </c>
     </row>
-    <row r="51" spans="1:10" s="1" customFormat="1">
+    <row r="51" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -10315,7 +10322,7 @@
         <v>Fetches a bundle of all Goal resources for the specified patient and start-date</v>
       </c>
     </row>
-    <row r="52" spans="1:10" s="1" customFormat="1">
+    <row r="52" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -10345,7 +10352,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="53" spans="1:10" s="1" customFormat="1">
+    <row r="53" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -10375,7 +10382,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="54" spans="1:10" s="1" customFormat="1">
+    <row r="54" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -10406,7 +10413,7 @@
         <v>Fetches a bundle of all MedicationStatement resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="55" spans="1:10" s="1" customFormat="1">
+    <row r="55" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -10436,7 +10443,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="56" spans="1:10" s="1" customFormat="1">
+    <row r="56" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -10467,7 +10474,7 @@
         <v>Fetches a bundle of all Procedure resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="57" spans="1:10" s="1" customFormat="1">
+    <row r="57" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -10498,7 +10505,7 @@
         <v>Fetches a bundle of all Procedure resources for the specified patient and date</v>
       </c>
     </row>
-    <row r="58" spans="1:10" s="1" customFormat="1">
+    <row r="58" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -10529,7 +10536,7 @@
         <v>Fetches a bundle of all Procedure resources for the specified patient and date and procedure code(s).  SHOULD support search by multiple codes.</v>
       </c>
     </row>
-    <row r="59" spans="1:10" s="1" customFormat="1">
+    <row r="59" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -10561,7 +10568,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="60" spans="1:10" s="1" customFormat="1">
+    <row r="60" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -10594,7 +10601,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and a category code = `laboratory`</v>
       </c>
     </row>
-    <row r="61" spans="1:10" s="1" customFormat="1">
+    <row r="61" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -10624,7 +10631,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and observation code(s).  SHOULD support search by multiple report codes. The Observation `code` parameter searches `Observation.code only.</v>
       </c>
     </row>
-    <row r="62" spans="1:10" s="1" customFormat="1">
+    <row r="62" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>61</v>
       </c>
@@ -10657,7 +10664,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and date and a category code = `laboratory`</v>
       </c>
     </row>
-    <row r="63" spans="1:10" s="1" customFormat="1">
+    <row r="63" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>62</v>
       </c>
@@ -10687,7 +10694,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="64" spans="1:10" s="1" customFormat="1">
+    <row r="64" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>63</v>
       </c>
@@ -10717,7 +10724,7 @@
         <v>Fetches a bundle of all !Observation resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="65" spans="1:16" s="1" customFormat="1">
+    <row r="65" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>58</v>
       </c>
@@ -10750,7 +10757,7 @@
         <v>Fetches a bundle of all CarePlan resources for the specified patient and category=`assess-plan`</v>
       </c>
     </row>
-    <row r="66" spans="1:16" s="1" customFormat="1">
+    <row r="66" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>59</v>
       </c>
@@ -10764,7 +10771,7 @@
         <v>214</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>81</v>
+        <v>13</v>
       </c>
       <c r="F66" s="1" t="s">
         <v>241</v>
@@ -10782,7 +10789,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="67" spans="1:16" s="1" customFormat="1">
+    <row r="67" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>61</v>
       </c>
@@ -10814,7 +10821,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="68" spans="1:16" s="1" customFormat="1">
+    <row r="68" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>62</v>
       </c>
@@ -10846,7 +10853,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="69" spans="1:16" s="1" customFormat="1">
+    <row r="69" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>63</v>
       </c>
@@ -10879,7 +10886,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="70" spans="1:16" ht="15.75">
+    <row r="70" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>64</v>
       </c>
@@ -10918,7 +10925,7 @@
       <c r="O70" s="1"/>
       <c r="P70" s="1"/>
     </row>
-    <row r="71" spans="1:16" s="1" customFormat="1">
+    <row r="71" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>58</v>
       </c>
@@ -10951,7 +10958,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and category and status</v>
       </c>
     </row>
-    <row r="72" spans="1:16" s="1" customFormat="1">
+    <row r="72" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>59</v>
       </c>
@@ -10984,7 +10991,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and a category code = `vital-signs`</v>
       </c>
     </row>
-    <row r="73" spans="1:16" s="1" customFormat="1">
+    <row r="73" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>60</v>
       </c>
@@ -11017,7 +11024,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and observation code(s).  SHOULD support search by multiple codes. The Observation `code` parameter searches `Observation.code only.</v>
       </c>
     </row>
-    <row r="74" spans="1:16" s="1" customFormat="1">
+    <row r="74" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>61</v>
       </c>
@@ -11050,7 +11057,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and date and a category code = `vital-signs`</v>
       </c>
     </row>
-    <row r="75" spans="1:16" s="1" customFormat="1">
+    <row r="75" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>62</v>
       </c>
@@ -11080,7 +11087,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and date and report code(s).  SHOULD support search by multiple codes.</v>
       </c>
     </row>
-    <row r="76" spans="1:16" s="1" customFormat="1">
+    <row r="76" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>39</v>
       </c>
@@ -11111,7 +11118,7 @@
         <v>Fetches a bundle of all DocumentReference resources for the specified patient and status. See the implementation notes above for how to access the actual document.</v>
       </c>
     </row>
-    <row r="77" spans="1:16" s="1" customFormat="1">
+    <row r="77" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>43</v>
       </c>
@@ -11140,7 +11147,7 @@
         <v>Fetches a bundle of all !DocumentReference resources for the specified patient and period. See the implementation notes above for how to access the actual document.</v>
       </c>
     </row>
-    <row r="78" spans="1:16" s="1" customFormat="1">
+    <row r="78" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>40</v>
       </c>
@@ -11173,7 +11180,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="79" spans="1:16" s="1" customFormat="1" ht="15.75">
+    <row r="79" spans="1:16" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>42</v>
       </c>
@@ -11206,7 +11213,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="80" spans="1:16" s="1" customFormat="1">
+    <row r="80" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>41</v>
       </c>
@@ -11236,7 +11243,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="81" spans="1:10" s="1" customFormat="1">
+    <row r="81" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>43</v>
       </c>
@@ -11267,7 +11274,7 @@
         <v>Fetches a bundle of all DocumentReference resources for the specified patient and type and period. See the implementation notes above for how to access the actual document.</v>
       </c>
     </row>
-    <row r="82" spans="1:10" s="1" customFormat="1">
+    <row r="82" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>41</v>
       </c>

</xml_diff>